<commit_message>
edit checklist to match ADEMP format
</commit_message>
<xml_diff>
--- a/Checklist/Checklist.xlsx
+++ b/Checklist/Checklist.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\4216318\Desktop\StandardizedEvaluation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\4216318\Desktop\StandardizedEvaluation\Checklist\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C6F3E66-19D6-4E68-AB17-096799C13DCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E02504B-9329-4158-8D69-48F419DC5EB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5520" yWindow="3825" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{69AEAAA5-9F04-4B14-9CC7-904BF5F66B11}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{69AEAAA5-9F04-4B14-9CC7-904BF5F66B11}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="71">
   <si>
     <t>2. Data generation</t>
   </si>
@@ -185,19 +186,96 @@
   </si>
   <si>
     <t>Reference method (e.g. complete case analysis)</t>
+  </si>
+  <si>
+    <t>Methods</t>
+  </si>
+  <si>
+    <t>Aims</t>
+  </si>
+  <si>
+    <t>Estimands</t>
+  </si>
+  <si>
+    <t>Performance measures</t>
+  </si>
+  <si>
+    <t>e.g. simulation scope</t>
+  </si>
+  <si>
+    <t>Data-generating mechanisms</t>
+  </si>
+  <si>
+    <t>e.g. data generation and missingness generation</t>
+  </si>
+  <si>
+    <t>missingness mechanisms (incl. type or functional form of the missing data model)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">missingness patterns (incl. missingness proportion) </t>
+  </si>
+  <si>
+    <t>data source (incl. model-based or design-based, sampling variance)</t>
+  </si>
+  <si>
+    <t>data characteristics (incl. multivariate relations and data structures such as clustering)</t>
+  </si>
+  <si>
+    <t>e.g. missing data methods and analytic method</t>
+  </si>
+  <si>
+    <t xml:space="preserve">imputation methods (incl. parameters such as the number of imputations) </t>
+  </si>
+  <si>
+    <t>estimation method (incl. reference methods such as complete case analysis)</t>
+  </si>
+  <si>
+    <t>□</t>
+  </si>
+  <si>
+    <t>e.g. evaluation of estimates and imputed values</t>
+  </si>
+  <si>
+    <t>e.g. complete data target</t>
+  </si>
+  <si>
+    <t>statistical properties (incl. comparative performance, if applicable)</t>
+  </si>
+  <si>
+    <t>validity of imputations (incl. imputation model fit and distributional characteristics)</t>
+  </si>
+  <si>
+    <t>simulation design (incl. pseudo-code or flow diagram)</t>
+  </si>
+  <si>
+    <t>required level of precision (incl. number of simulation repetitions)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -208,7 +286,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -216,13 +294,56 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -543,142 +664,142 @@
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="1" max="1" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
         <v>8</v>
       </c>
@@ -692,16 +813,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1ABEC980-E659-4E2E-ABA5-C2C5C27401BA}">
   <dimension ref="A2:B24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.5703125" customWidth="1"/>
+    <col min="1" max="1" width="4.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -709,22 +830,22 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>2</v>
       </c>
@@ -732,27 +853,27 @@
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>3</v>
       </c>
@@ -760,17 +881,17 @@
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>4</v>
       </c>
@@ -778,22 +899,22 @@
         <v>37</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>5</v>
       </c>
@@ -801,22 +922,22 @@
         <v>40</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>6</v>
       </c>
@@ -824,12 +945,12 @@
         <v>44</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
         <v>46</v>
       </c>
@@ -837,4 +958,184 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D1A0382-B509-4614-A961-CF37D2CD6BBD}">
+  <dimension ref="A2:C22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="2.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="40.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="71.88671875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="C2" s="9"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="2"/>
+      <c r="B3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B4" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B5" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C5" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C6" s="6"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="2"/>
+      <c r="B7" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B8" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C8" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B9" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C9" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B10" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C10" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B11" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C11" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C12" s="6"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="2"/>
+      <c r="B13" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C14" s="6"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" s="2"/>
+      <c r="B15" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B16" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C16" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B17" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C17" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C18" s="6"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" s="2"/>
+      <c r="B19" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B20" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C20" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" s="10"/>
+      <c r="B21" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="C21" s="10" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B22" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update checklist in manuscript
</commit_message>
<xml_diff>
--- a/Checklist/Checklist.xlsx
+++ b/Checklist/Checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\4216318\Desktop\StandardizedEvaluation\Checklist\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7BAD622-00E0-4DFE-AD3C-A22BE2C5DA13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4208A275-C607-4AD5-AB43-2A904704802C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{69AEAAA5-9F04-4B14-9CC7-904BF5F66B11}"/>
   </bookViews>
@@ -504,7 +504,7 @@
   <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A2" sqref="A2:B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.4" zeroHeight="1" x14ac:dyDescent="0.3"/>

</xml_diff>